<commit_message>
Projectile fix + csv fix
</commit_message>
<xml_diff>
--- a/Rational_Level_Design.xlsx
+++ b/Rational_Level_Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE17732A-8024-4BA6-BBE4-40D90D4454ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351ED301-138A-45DB-9A09-27B73071D70C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LD" sheetId="1" r:id="rId1"/>
@@ -2364,8 +2364,8 @@
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2686,7 +2686,7 @@
       <c r="L11" s="73"/>
       <c r="M11" s="73"/>
       <c r="N11" s="61" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O11" s="44"/>
       <c r="P11" s="128"/>
@@ -2708,7 +2708,7 @@
       <c r="L12" s="79"/>
       <c r="M12" s="79"/>
       <c r="N12" s="61" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O12" s="44"/>
       <c r="P12" s="128"/>
@@ -2732,7 +2732,7 @@
         <v>55</v>
       </c>
       <c r="N13" s="61" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O13" s="44"/>
       <c r="P13" s="128"/>
@@ -2756,7 +2756,7 @@
         <v>51</v>
       </c>
       <c r="N14" s="61" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O14" s="44"/>
       <c r="P14" s="128"/>
@@ -2778,7 +2778,7 @@
       <c r="L15" s="79"/>
       <c r="M15" s="79"/>
       <c r="N15" s="61" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="128"/>

</xml_diff>

<commit_message>
JD Progress and other random stuff
</commit_message>
<xml_diff>
--- a/Rational_Level_Design.xlsx
+++ b/Rational_Level_Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B0717F-E0D0-4732-8A29-6D96E72FD399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4B4653-E967-441F-AAA3-CF1B1D69C85D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2364,8 +2364,8 @@
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2568,7 +2568,7 @@
         <v>51</v>
       </c>
       <c r="N7" s="61" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O7" s="23"/>
       <c r="P7" s="23"/>
@@ -2686,7 +2686,7 @@
       <c r="L11" s="73"/>
       <c r="M11" s="73"/>
       <c r="N11" s="61" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="44"/>
       <c r="P11" s="128"/>
@@ -2708,7 +2708,7 @@
       <c r="L12" s="79"/>
       <c r="M12" s="79"/>
       <c r="N12" s="61" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="44"/>
       <c r="P12" s="128"/>
@@ -2732,7 +2732,7 @@
         <v>55</v>
       </c>
       <c r="N13" s="61" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="44"/>
       <c r="P13" s="128"/>
@@ -2756,7 +2756,7 @@
         <v>51</v>
       </c>
       <c r="N14" s="61" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="44"/>
       <c r="P14" s="128"/>
@@ -2778,7 +2778,7 @@
       <c r="L15" s="79"/>
       <c r="M15" s="79"/>
       <c r="N15" s="61" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="128"/>
@@ -3045,7 +3045,7 @@
         <v>51</v>
       </c>
       <c r="N25" s="61" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O25" s="138" t="s">
         <v>58</v>
@@ -3069,7 +3069,7 @@
       <c r="L26" s="79"/>
       <c r="M26" s="79"/>
       <c r="N26" s="61" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O26" s="139"/>
       <c r="P26" s="125"/>
@@ -3093,7 +3093,7 @@
         <v>53</v>
       </c>
       <c r="N27" s="61" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O27" s="139"/>
       <c r="P27" s="125"/>
@@ -3115,7 +3115,7 @@
       <c r="L28" s="79"/>
       <c r="M28" s="79"/>
       <c r="N28" s="61" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O28" s="139"/>
       <c r="P28" s="125"/>
@@ -3137,7 +3137,7 @@
       <c r="L29" s="79"/>
       <c r="M29" s="79"/>
       <c r="N29" s="61" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O29" s="140"/>
       <c r="P29" s="125"/>

</xml_diff>